<commit_message>
questions and student excel sheets done
</commit_message>
<xml_diff>
--- a/Questions_data.xlsx
+++ b/Questions_data.xlsx
@@ -6,13 +6,65 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Student Data" r:id="rId3" sheetId="1"/>
+    <sheet name="Question" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>how are you ?</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>MCQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">want to sleep </t>
+  </si>
+  <si>
+    <t>fine</t>
+  </si>
+  <si>
+    <t>not fine</t>
+  </si>
+  <si>
+    <t>IDK</t>
+  </si>
+  <si>
+    <t>May I ask you a question?</t>
+  </si>
+  <si>
+    <t>OfCourse</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Why Not?</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,12 +107,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="n" s="0">
+        <v>79.0</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>80.0</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>81.0</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>